<commit_message>
Update execution time python
</commit_message>
<xml_diff>
--- a/RQ1_Results/aggregated/valuecorrelation.xlsx
+++ b/RQ1_Results/aggregated/valuecorrelation.xlsx
@@ -472,7 +472,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,6 +796,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010093600FF255B683488FA7D78A61F6ACA2" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f3e773d715c6b3174e4c142805127174">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c7f76cb1-89ee-4b57-9b7d-f2588e6f8ef3" xmlns:ns4="0e7fdb95-cc9f-47aa-82a3-a3229e5912eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03a8284b1319d4c8f050bc920eb60756" ns3:_="" ns4:_="">
     <xsd:import namespace="c7f76cb1-89ee-4b57-9b7d-f2588e6f8ef3"/>
@@ -1004,22 +1019,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70FD6778-C405-40BA-8CE6-6E2D6BFC385E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A3AB2B4-78D6-4DE4-9CF3-707166797880}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2F798B0-6C91-490F-B3A7-7F21C5075544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1036,21 +1053,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A3AB2B4-78D6-4DE4-9CF3-707166797880}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70FD6778-C405-40BA-8CE6-6E2D6BFC385E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>